<commit_message>
Fix elxflash name in ECD config.
</commit_message>
<xml_diff>
--- a/17A-Red-ECD-BOM-06-29.xlsx
+++ b/17A-Red-ECD-BOM-06-29.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="UX Package Info" sheetId="5" r:id="rId1"/>
@@ -1652,6 +1652,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1665,24 +1683,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="336">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2345,38 +2345,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="90" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="84"/>
+      <c r="B1" s="90"/>
       <c r="C1" s="67"/>
       <c r="D1" s="67"/>
     </row>
     <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="90" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="84"/>
+      <c r="B2" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="86" t="s">
         <v>178</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2419,20 +2419,20 @@
         <v>202</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="88" t="s">
+      <c r="H6" s="83" t="s">
         <v>206</v>
       </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="83"/>
       <c r="N6" s="20"/>
       <c r="O6" s="52"/>
       <c r="P6" s="21"/>
@@ -2549,14 +2549,14 @@
         <v>4</v>
       </c>
       <c r="G10" s="27"/>
-      <c r="H10" s="88" t="s">
+      <c r="H10" s="83" t="s">
         <v>205</v>
       </c>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
       <c r="O10" s="52"/>
       <c r="P10" s="26"/>
     </row>
@@ -2575,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="30"/>
-      <c r="H11" s="89" t="s">
+      <c r="H11" s="84" t="s">
         <v>263</v>
       </c>
       <c r="I11" s="59" t="s">
@@ -2611,7 +2611,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="25"/>
-      <c r="H12" s="90"/>
+      <c r="H12" s="85"/>
       <c r="I12" s="59" t="s">
         <v>195</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="25"/>
-      <c r="H13" s="89" t="s">
+      <c r="H13" s="84" t="s">
         <v>264</v>
       </c>
       <c r="I13" s="59" t="s">
@@ -2680,7 +2680,7 @@
       <c r="F14" s="24">
         <v>8</v>
       </c>
-      <c r="H14" s="90"/>
+      <c r="H14" s="85"/>
       <c r="I14" s="59" t="s">
         <v>253</v>
       </c>
@@ -2721,11 +2721,11 @@
         <v>211</v>
       </c>
       <c r="C16" s="31"/>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="80" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="82"/>
       <c r="O16" s="52"/>
       <c r="P16" s="26"/>
     </row>
@@ -3081,16 +3081,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="H6:M6"/>
     <mergeCell ref="H10:M10"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>